<commit_message>
Changes in Transfer In patient script
</commit_message>
<xml_diff>
--- a/Agedcare.xlsx
+++ b/Agedcare.xlsx
@@ -5,24 +5,25 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Table Data" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Configuration" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Signature" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Data" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="81">
   <si>
     <t xml:space="preserve">Transaction ID</t>
   </si>
@@ -253,6 +254,18 @@
   </si>
   <si>
     <t xml:space="preserve">valeshan.naidoo@strongroom.ai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added By Mayur</t>
   </si>
 </sst>
 </file>
@@ -262,7 +275,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -288,16 +301,41 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -309,7 +347,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -333,8 +371,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -359,15 +400,88 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Bad" xfId="20"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF9C0006"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFC7CE"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -378,11 +492,11 @@
   </sheetPr>
   <dimension ref="B1:N19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.15"/>
@@ -397,7 +511,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="24.49"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +552,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -473,7 +587,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
@@ -508,7 +622,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
@@ -543,7 +657,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
@@ -578,7 +692,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
         <v>33</v>
       </c>
@@ -613,7 +727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
         <v>37</v>
       </c>
@@ -648,7 +762,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
         <v>41</v>
       </c>
@@ -683,7 +797,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
         <v>44</v>
       </c>
@@ -718,7 +832,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
         <v>47</v>
       </c>
@@ -753,7 +867,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
         <v>49</v>
       </c>
@@ -788,7 +902,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
         <v>52</v>
       </c>
@@ -823,7 +937,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
         <v>55</v>
       </c>
@@ -858,7 +972,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
         <v>58</v>
       </c>
@@ -893,7 +1007,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
         <v>62</v>
       </c>
@@ -928,7 +1042,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
         <v>65</v>
       </c>
@@ -963,13 +1077,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="2"/>
     </row>
   </sheetData>
@@ -991,19 +1105,20 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.86"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>69</v>
       </c>
@@ -1020,7 +1135,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>73</v>
       </c>
@@ -1056,17 +1171,17 @@
   <dimension ref="B1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.72"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
         <v>74</v>
       </c>
@@ -1074,7 +1189,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="s">
         <v>76</v>
       </c>
@@ -1094,4 +1209,157 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="42.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="30.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.29"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>1111</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="valeshan.naidoo@strongroom.ai"/>
+    <hyperlink ref="H3" r:id="rId2" display="valeshan.naidoo@strongroom.ai"/>
+    <hyperlink ref="H4" r:id="rId3" display="valeshan.naidoo@strongroom.ai"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated code for stock test case for 0 quantity
updated code for stock test case for 0 quantity
</commit_message>
<xml_diff>
--- a/Agedcare.xlsx
+++ b/Agedcare.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="85">
   <si>
     <t xml:space="preserve">Transaction ID</t>
   </si>
@@ -265,13 +265,10 @@
     <t xml:space="preserve">Note</t>
   </si>
   <si>
-    <t xml:space="preserve">Transfer in Imprest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quinapril 10 mg tablet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anthony Jones</t>
+    <t xml:space="preserve">Transfer out Imprest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acetec 5 mg tablet</t>
   </si>
   <si>
     <t xml:space="preserve">Added Note</t>
@@ -280,7 +277,7 @@
     <t xml:space="preserve">1111</t>
   </si>
   <si>
-    <t xml:space="preserve">Transfer out Imprest</t>
+    <t xml:space="preserve">Endone 5 mg tablet</t>
   </si>
 </sst>
 </file>
@@ -513,7 +510,7 @@
       <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.15"/>
@@ -1122,10 +1119,10 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.86"/>
@@ -1191,7 +1188,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.65"/>
@@ -1236,10 +1233,10 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.85"/>
@@ -1291,46 +1288,45 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>74</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>84</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>74</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated file for invalid drugname test case
Updated file for invalid drugname test case
excell ,
Transfer in imprest
Transfer in Patient
Transfer out imprest
Transfer out patient
</commit_message>
<xml_diff>
--- a/Agedcare.xlsx
+++ b/Agedcare.xlsx
@@ -265,10 +265,10 @@
     <t xml:space="preserve">Note</t>
   </si>
   <si>
-    <t xml:space="preserve">Transfer out Imprest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acetec 5 mg tablet</t>
+    <t xml:space="preserve">Transfer out Patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hmhhm</t>
   </si>
   <si>
     <t xml:space="preserve">Added Note</t>
@@ -277,7 +277,7 @@
     <t xml:space="preserve">1111</t>
   </si>
   <si>
-    <t xml:space="preserve">Endone 5 mg tablet</t>
+    <t xml:space="preserve">mhmhm</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
       <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.15"/>
@@ -1122,7 +1122,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.86"/>
@@ -1188,7 +1188,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.65"/>
@@ -1233,10 +1233,10 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.85"/>

</xml_diff>

<commit_message>
transfer in imprest and patient addded by parth
</commit_message>
<xml_diff>
--- a/Agedcare.xlsx
+++ b/Agedcare.xlsx
@@ -245,15 +245,15 @@
     <t>https://staging.strongroom.ai/login</t>
   </si>
   <si>
+    <t>valeshan.naidoo@strongroom.ai</t>
+  </si>
+  <si>
     <t>Username</t>
   </si>
   <si>
     <t>PIN/Password</t>
   </si>
   <si>
-    <t>valeshan.naidoo@strongroom.ai</t>
-  </si>
-  <si>
     <t>Action</t>
   </si>
   <si>
@@ -263,10 +263,13 @@
     <t>Note</t>
   </si>
   <si>
-    <t>Transfer in Imprest</t>
-  </si>
-  <si>
-    <t>alprazolam 1 mg tablet</t>
+    <t>Transfer in Patient</t>
+  </si>
+  <si>
+    <t>Morphine Sulfate (DBL) 15 mg/mL injection, ampoule</t>
+  </si>
+  <si>
+    <t>Nancy Holt</t>
   </si>
   <si>
     <t>Added Note</t>
@@ -275,62 +278,14 @@
     <t>1111</t>
   </si>
   <si>
-    <t>Transfer in Patient</t>
-  </si>
-  <si>
-    <t>Transfer out Imprest</t>
-  </si>
-  <si>
-    <t>6e26790f-e97b-47a9-978b-e42b5915acbc</t>
-  </si>
-  <si>
-    <t>Transfer out Patient</t>
-  </si>
-  <si>
-    <t>7e26790f-e97b-47a9-978b-e42b5915acbc</t>
-  </si>
-  <si>
-    <t>John Demo</t>
-  </si>
-  <si>
-    <t>Destroy imprest</t>
-  </si>
-  <si>
-    <t>prilocaine hydrochloride 1% (50 mg/5 mL) injection, ampoule</t>
-  </si>
-  <si>
-    <t>8e26790f-e97b-47a9-978b-e42b5915acbc</t>
-  </si>
-  <si>
-    <t>Destroy Patient</t>
-  </si>
-  <si>
-    <t>(rufinamide) Inovelon 200 mg tablet</t>
-  </si>
-  <si>
-    <t>9e26790f-e97b-47a9-978b-e42b5915acbc</t>
-  </si>
-  <si>
-    <t>Nancy Holt</t>
-  </si>
-  <si>
-    <t>Outgoing imprest</t>
-  </si>
-  <si>
-    <t>10e26790f-e97b-47a9-978b-e42b5915acbc</t>
-  </si>
-  <si>
-    <t>Outgoing Patient</t>
-  </si>
-  <si>
-    <t>11e26790f-e97b-47a9-978b-e42b5915acbc</t>
+    <t>Endone 5 mg tablet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -365,11 +320,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -385,31 +335,14 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <left>
-        <color indexed="64"/>
-      </left>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top>
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-      <diagonal>
-        <color indexed="64"/>
-      </diagonal>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -425,12 +358,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,7 +730,7 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="12.19141" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="5.7" customWidth="1"/>
     <col min="2" max="2" width="35.15" customWidth="1"/>
@@ -1407,10 +1334,10 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.30859" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="12.54297" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="31.57" customWidth="1"/>
     <col min="2" max="2" width="17.86" customWidth="1"/>
@@ -1437,7 +1364,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="12.8">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1445,7 +1372,7 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -1471,7 +1398,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94141" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="12.17188" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="12.78" customWidth="1"/>
     <col min="2" max="2" width="27.65" customWidth="1"/>
@@ -1480,15 +1407,15 @@
   <sheetData>
     <row r="1">
       <c r="B1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C2" s="5">
         <v>1111</v>
@@ -1511,18 +1438,18 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="A1:XFD1048576"/>
+      <selection activeCell="E4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.824219" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.72266" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="19.71" customWidth="1"/>
-    <col min="2" max="2" width="25.14" customWidth="1"/>
-    <col min="3" max="5" width="42.71" customWidth="1"/>
-    <col min="6" max="6" width="10.42" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="30.28" customWidth="1"/>
-    <col min="9" max="9" width="17.29" customWidth="1"/>
+    <col min="1" max="1" width="18.85547" customWidth="1"/>
+    <col min="3" max="3" width="60.85" customWidth="1"/>
+    <col min="4" max="4" width="20.56" customWidth="1"/>
+    <col min="5" max="5" width="18.06" customWidth="1"/>
+    <col min="7" max="7" width="13.06" customWidth="1"/>
+    <col min="8" max="8" width="27.92" customWidth="1"/>
+    <col min="9" max="9" width="16.81" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75">
@@ -1548,235 +1475,76 @@
         <v>79</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" ht="15">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11">
-        <v>2</v>
-      </c>
-      <c r="G2" s="11" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" s="9" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" ht="15">
+      <c r="H2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="11">
-        <v>2</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" ht="15">
-      <c r="A4" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11">
-        <v>2</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" ht="15">
-      <c r="A5" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="11">
-        <v>2</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" ht="15">
-      <c r="A6" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11">
-        <v>2</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" ht="15">
-      <c r="A7" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" s="11">
-        <v>2</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" ht="15">
-      <c r="A8" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11">
-        <v>2</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I8" s="9">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="9" ht="15">
-      <c r="A9" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="11">
-        <v>2</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A9">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2:A3">
       <formula1>"Outgoing Patient,Outgoing imprest,Destroy Patient,Destroy imprest,Transfer out Patient,Transfer out Imprest,Transfer in Patient,Transfer in Imprest"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7479166" right="0.7479166" top="0.9840278" bottom="0.9840278" header="0.5118055" footer="0.5118055"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.052778" bottom="1.052778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>